<commit_message>
PPT e ajustes na arquitetura
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de Backlog.xlsx
+++ b/Documentação/Planilha de Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fecco\OneDrive\Área de Trabalho\project-hunter\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08d7f3c16d54179/Área de Trabalho/Projeto/project-hunter/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D0837A-3B31-4BF7-8E8D-02E5A5105A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{871AB88A-CFCB-4751-B4F7-9013E6C36C98}"/>
+    <workbookView minimized="1" xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{871AB88A-CFCB-4751-B4F7-9013E6C36C98}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -293,6 +293,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,9 +303,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684ACFEA-3688-451E-BB92-085602F58954}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,386 +648,346 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="5">
         <v>5</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <f>SUM('Sprint Backlog'!D2:D5)</f>
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <f>SUM('Sprint Backlog'!D6:D10)</f>
         <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <f>SUM('Sprint Backlog'!D11:D14)</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <f>SUM('Sprint Backlog'!D15:D17)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <f>SUM('Sprint Backlog'!D18:D21)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="5">
         <v>6</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>4</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <f>SUM('Sprint Backlog'!D22:D23)</f>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="A18" s="5">
         <v>7</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>5</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <f>SUM('Sprint Backlog'!D24:D26)</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="5">
         <v>8</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <f>SUM('Sprint Backlog'!D27:D29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
+      <c r="A24" s="5">
         <v>9</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="5">
         <v>3</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <f>SUM('Sprint Backlog'!D30:D33)</f>
         <v>10.5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="7"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
+      <c r="A26" s="5">
         <v>10</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="5">
         <v>2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <f>SUM('Sprint Backlog'!D34:D37)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="7"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="8">
+      <c r="A29" s="5">
         <v>11</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>2</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <f>SUM('Sprint Backlog'!D38:D41)</f>
         <v>5.25</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="7"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
+      <c r="A32" s="5">
         <v>12</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="5">
         <v>5</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <f>SUM('Sprint Backlog'!D42:D48)</f>
         <v>13.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
+      <c r="A36" s="6">
         <v>13</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="6">
         <v>5</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <f>SUM('Sprint Backlog'!D49:D53)</f>
         <v>10.5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="C36:C38"/>
@@ -1040,6 +1000,46 @@
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="D32:D35"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1049,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0B18D4-338A-4F5F-841C-BE448931BD93}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -1084,13 +1084,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="5">
         <v>5</v>
       </c>
       <c r="D2" s="2">
@@ -1104,9 +1104,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="2">
         <v>2</v>
       </c>
@@ -1118,9 +1118,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="2">
         <v>3</v>
       </c>
@@ -1132,9 +1132,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="2">
         <v>1</v>
       </c>
@@ -1146,13 +1146,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>5</v>
       </c>
       <c r="D6" s="2">
@@ -1166,9 +1166,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="2">
         <v>2</v>
       </c>
@@ -1180,9 +1180,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="2">
         <v>3</v>
       </c>
@@ -1194,9 +1194,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="2">
         <v>2</v>
       </c>
@@ -1208,9 +1208,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="2">
         <v>1</v>
       </c>
@@ -1222,13 +1222,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>4</v>
       </c>
       <c r="D11" s="2">
@@ -1242,9 +1242,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="2">
         <v>3</v>
       </c>
@@ -1256,9 +1256,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="2">
         <v>2</v>
       </c>
@@ -1270,9 +1270,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="2">
         <v>1</v>
       </c>
@@ -1284,13 +1284,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="A15" s="6">
         <v>4</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>4</v>
       </c>
       <c r="D15" s="2">
@@ -1304,9 +1304,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="2">
         <v>1</v>
       </c>
@@ -1318,9 +1318,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="2">
         <v>0.5</v>
       </c>
@@ -1332,13 +1332,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
+      <c r="A18" s="6">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>3</v>
       </c>
       <c r="D18" s="2">
@@ -1352,9 +1352,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="2">
         <v>0.5</v>
       </c>
@@ -1366,9 +1366,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="2">
         <v>1</v>
       </c>
@@ -1380,9 +1380,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="2">
         <v>0.5</v>
       </c>
@@ -1394,13 +1394,13 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22" s="6">
         <v>6</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>4</v>
       </c>
       <c r="D22" s="2">
@@ -1414,9 +1414,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="2">
         <v>0.5</v>
       </c>
@@ -1428,13 +1428,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
+      <c r="A24" s="5">
         <v>7</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="5">
         <v>5</v>
       </c>
       <c r="D24" s="2">
@@ -1448,9 +1448,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="2">
         <v>3</v>
       </c>
@@ -1462,9 +1462,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="2">
         <v>0.5</v>
       </c>
@@ -1476,13 +1476,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
+      <c r="A27" s="5">
         <v>8</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="5">
         <v>4</v>
       </c>
       <c r="D27" s="2"/>
@@ -1490,29 +1490,29 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="8">
+      <c r="A30" s="5">
         <v>9</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="5">
         <v>3</v>
       </c>
       <c r="D30" s="2">
@@ -1526,9 +1526,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="2">
         <v>2</v>
       </c>
@@ -1540,9 +1540,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="2">
         <v>1.5</v>
       </c>
@@ -1554,9 +1554,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="2">
         <v>1</v>
       </c>
@@ -1568,13 +1568,13 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
+      <c r="A34" s="5">
         <v>10</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="5">
         <v>3</v>
       </c>
       <c r="D34" s="2">
@@ -1588,9 +1588,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="2">
         <v>2</v>
       </c>
@@ -1602,9 +1602,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="2">
         <v>1</v>
       </c>
@@ -1616,9 +1616,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="2">
         <v>0.5</v>
       </c>
@@ -1630,13 +1630,13 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="8">
+      <c r="A38" s="5">
         <v>11</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="5">
         <v>2</v>
       </c>
       <c r="D38" s="2">
@@ -1650,9 +1650,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="2">
         <v>2.5</v>
       </c>
@@ -1664,9 +1664,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
       <c r="D40" s="2">
         <v>0.75</v>
       </c>
@@ -1678,9 +1678,9 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
       <c r="D41" s="2">
         <v>0.5</v>
       </c>
@@ -1692,13 +1692,13 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
+      <c r="A42" s="6">
         <v>12</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="6">
         <v>5</v>
       </c>
       <c r="D42" s="2">
@@ -1712,9 +1712,9 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
       <c r="D43" s="2">
         <v>2</v>
       </c>
@@ -1726,9 +1726,9 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="2">
         <v>2</v>
       </c>
@@ -1740,9 +1740,9 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
       <c r="D45" s="2">
         <v>1.5</v>
       </c>
@@ -1754,9 +1754,9 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
       <c r="D46" s="2">
         <v>2</v>
       </c>
@@ -1768,9 +1768,9 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
       <c r="D47" s="2">
         <v>2.5</v>
       </c>
@@ -1782,9 +1782,9 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="2">
         <v>1</v>
       </c>
@@ -1796,13 +1796,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+      <c r="A49" s="6">
         <v>13</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="6">
         <v>5</v>
       </c>
       <c r="D49" s="2">
@@ -1816,9 +1816,9 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
       <c r="D50" s="2">
         <v>1.5</v>
       </c>
@@ -1830,9 +1830,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="2">
         <v>2</v>
       </c>
@@ -1844,9 +1844,9 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="2">
         <v>2.5</v>
       </c>
@@ -1858,9 +1858,9 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="2">
         <v>2.5</v>
       </c>
@@ -1873,6 +1873,30 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C42:C48"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
@@ -1888,30 +1912,6 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
-    <mergeCell ref="C42:C48"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="C38:C41"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>